<commit_message>
pgm1 & 3 commit
</commit_message>
<xml_diff>
--- a/DSA_PRACTICE/dsa_practice/src/main/java/com/dsa/FINAL450.xlsx
+++ b/DSA_PRACTICE/dsa_practice/src/main/java/com/dsa/FINAL450.xlsx
@@ -1859,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B94" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="B103" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2428,7 +2428,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="21">
@@ -2461,7 +2461,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="21">
@@ -2917,7 +2917,7 @@
         <v>99</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="21">
@@ -3005,7 +3005,7 @@
         <v>107</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="21">

</xml_diff>